<commit_message>
Update web reports - 2025-10-25 23:17:01
</commit_message>
<xml_diff>
--- a/quickbook_summary.xlsx
+++ b/quickbook_summary.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -467,12 +467,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="28" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -876,6 +876,150 @@
       </c>
       <c r="H11" s="5" t="n">
         <v>200</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>4001 · Service Income</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Invoice</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>NGSJ25-003</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>Materials, Fittings, and Equipment</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>1100 · Trade Debtors</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>312198.51</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>4003 · Mobilization Income</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Invoice</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>NGSJ25-003</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>Premob support, Management, &amp; Technical Direction</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>1100 · Trade Debtors</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>9827.1</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>4003 · Mobilization Income</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Invoice</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>NGSJ25-003</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>Procurement/Logistics</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>1100 · Trade Debtors</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>9100</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>4003 · Mobilization Income</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Invoice</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>NGSJ25-003</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>Equipment fabrication and prep, test, &amp; tune</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>1100 · Trade Debtors</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>27560</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -889,7 +1033,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -986,43 +1130,43 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45757</v>
+        <v>45756</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>5107.1 · Travel - Car Rental</t>
+          <t>1100 · Trade Debtors</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Credit Card Charge</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr"/>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>RENTER'S NAME: BRIAN MORRIS</t>
-        </is>
-      </c>
+          <t>Invoice</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>NGSJ25-001</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>2321 · Commerce Bank - Enterprise Acct</t>
+          <t>-SPLIT-</t>
         </is>
       </c>
       <c r="G3" s="4" t="n">
-        <v>209.92</v>
+        <v>51408</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45758</v>
+        <v>45757</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5107.1 · Travel - Car Rental</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -1030,23 +1174,19 @@
           <t>Credit Card Charge</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>BM</t>
-        </is>
-      </c>
+      <c r="D4" s="3" t="inlineStr"/>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>User: Brian Morris | Jobs: NO JOB | GL Accounts: 5111 Â· Parts &amp; material costs | Notes: Paint t...</t>
+          <t>RENTER'S NAME: BRIAN MORRIS</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>Credit Card at Wells Fargo Ban</t>
+          <t>2321 · Commerce Bank - Enterprise Acct</t>
         </is>
       </c>
       <c r="G4" s="4" t="n">
-        <v>37.03</v>
+        <v>209.92</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>300</v>
@@ -1054,11 +1194,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45759</v>
+        <v>45758</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>5107 · Travel - Other (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -1073,7 +1213,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>User: Brian Morris | Jobs: NO JOB | GL Accounts: 5107 Â· Travel - Other | Notes: San jose hotel ...</t>
+          <t>User: Brian Morris | Jobs: NO JOB | GL Accounts: 5111 Â· Parts &amp; material costs | Notes: Paint t...</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
@@ -1082,7 +1222,7 @@
         </is>
       </c>
       <c r="G5" s="4" t="n">
-        <v>18</v>
+        <v>37.03</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>300</v>
@@ -1090,11 +1230,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45795</v>
+        <v>45759</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5107 · Travel - Other (Direct)</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -1104,12 +1244,12 @@
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>BM</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>User: Sepehr Ghahremani | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5111 Â· Parts &amp; materia...</t>
+          <t>User: Brian Morris | Jobs: NO JOB | GL Accounts: 5107 Â· Travel - Other | Notes: San jose hotel ...</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
@@ -1118,7 +1258,7 @@
         </is>
       </c>
       <c r="G6" s="4" t="n">
-        <v>763.61</v>
+        <v>18</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>300</v>
@@ -1126,7 +1266,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45800</v>
+        <v>45795</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -1154,7 +1294,7 @@
         </is>
       </c>
       <c r="G7" s="4" t="n">
-        <v>178.98</v>
+        <v>763.61</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>300</v>
@@ -1162,11 +1302,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45852</v>
+        <v>45800</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>5105 · Travel - Airfare (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -1174,19 +1314,23 @@
           <t>Credit Card Charge</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr"/>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>Gordon Doull &amp; Vu T	Flight- SNA to SJC- SJC to SNA 7/17</t>
+          <t>User: Sepehr Ghahremani | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5111 Â· Parts &amp; materia...</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>2310 · American Express Delta</t>
+          <t>Credit Card at Wells Fargo Ban</t>
         </is>
       </c>
       <c r="G8" s="4" t="n">
-        <v>770.95</v>
+        <v>178.98</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>300</v>
@@ -1226,11 +1370,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45855</v>
+        <v>45852</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>5107.1 · Travel - Car Rental</t>
+          <t>5105 · Travel - Airfare (Direct)</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -1238,23 +1382,19 @@
           <t>Credit Card Charge</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>GD</t>
-        </is>
-      </c>
+      <c r="D10" s="3" t="inlineStr"/>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>Gordon Doull San Jose 7/17 - 7/17</t>
+          <t>Gordon Doull &amp; Vu T	Flight- SNA to SJC- SJC to SNA 7/17</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>2321 · Commerce Bank - Enterprise Acct</t>
+          <t>2310 · American Express Delta</t>
         </is>
       </c>
       <c r="G10" s="4" t="n">
-        <v>64.45</v>
+        <v>770.95</v>
       </c>
       <c r="H10" s="5" t="n">
         <v>300</v>
@@ -1262,11 +1402,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45856</v>
+        <v>45855</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>5105 · Travel - Airfare (Direct)</t>
+          <t>5107.1 · Travel - Car Rental</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -1276,21 +1416,21 @@
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>User: Vu Tran | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5105 Â· Travel - Airfare | Card: ...</t>
+          <t>Gordon Doull San Jose 7/17 - 7/17</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>Credit Card at Wells Fargo Ban</t>
+          <t>2321 · Commerce Bank - Enterprise Acct</t>
         </is>
       </c>
       <c r="G11" s="4" t="n">
-        <v>27.14</v>
+        <v>64.45</v>
       </c>
       <c r="H11" s="5" t="n">
         <v>300</v>
@@ -1298,11 +1438,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45857</v>
+        <v>45856</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>5107 · Travel - Other (Direct)</t>
+          <t>5105 · Travel - Airfare (Direct)</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -1312,12 +1452,12 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>VT</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>User: Gordon Doull | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5107 Â· Travel - Other | Not...</t>
+          <t>User: Vu Tran | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5105 Â· Travel - Airfare | Card: ...</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
@@ -1326,7 +1466,7 @@
         </is>
       </c>
       <c r="G12" s="4" t="n">
-        <v>30</v>
+        <v>27.14</v>
       </c>
       <c r="H12" s="5" t="n">
         <v>300</v>
@@ -1334,11 +1474,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45860</v>
+        <v>45857</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>5124 · License and permits (Direct)</t>
+          <t>5107 · Travel - Other (Direct)</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -1353,7 +1493,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>User: Gordon Doull | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5124 Â· License and permits ...</t>
+          <t>User: Gordon Doull | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5107 Â· Travel - Other | Not...</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
@@ -1362,7 +1502,7 @@
         </is>
       </c>
       <c r="G13" s="4" t="n">
-        <v>500</v>
+        <v>30</v>
       </c>
       <c r="H13" s="5" t="n">
         <v>300</v>
@@ -1370,35 +1510,35 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45873</v>
+        <v>45860</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5124 · License and permits (Direct)</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>Credit Card Charge</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>(E)429605</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>3 X 2 STD WELD CONC RED</t>
+          <t>User: Gordon Doull | Jobs: NGSJ - Northgate San Jose | GL Accounts: 5124 Â· License and permits ...</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>Credit Card at Wells Fargo Ban</t>
         </is>
       </c>
       <c r="G14" s="4" t="n">
-        <v>232.77</v>
+        <v>500</v>
       </c>
       <c r="H14" s="5" t="n">
         <v>300</v>
@@ -1425,7 +1565,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>3 STD WELD CAP</t>
+          <t>3 X 2 STD WELD CONC RED</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
@@ -1434,7 +1574,7 @@
         </is>
       </c>
       <c r="G15" s="4" t="n">
-        <v>92.11</v>
+        <v>232.77</v>
       </c>
       <c r="H15" s="5" t="n">
         <v>300</v>
@@ -1461,7 +1601,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>5 STD WELD CAP</t>
+          <t>3 STD WELD CAP</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
@@ -1470,7 +1610,7 @@
         </is>
       </c>
       <c r="G16" s="4" t="n">
-        <v>626.46</v>
+        <v>92.11</v>
       </c>
       <c r="H16" s="5" t="n">
         <v>300</v>
@@ -1497,7 +1637,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>2  STD WELD CAP</t>
+          <t>5 STD WELD CAP</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
@@ -1506,7 +1646,7 @@
         </is>
       </c>
       <c r="G17" s="4" t="n">
-        <v>305.11</v>
+        <v>626.46</v>
       </c>
       <c r="H17" s="5" t="n">
         <v>300</v>
@@ -1533,7 +1673,7 @@
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>Delivery</t>
+          <t>2  STD WELD CAP</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
@@ -1542,7 +1682,7 @@
         </is>
       </c>
       <c r="G18" s="4" t="n">
-        <v>15</v>
+        <v>305.11</v>
       </c>
       <c r="H18" s="5" t="n">
         <v>300</v>
@@ -1569,7 +1709,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>tax</t>
+          <t>Delivery</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
@@ -1578,7 +1718,7 @@
         </is>
       </c>
       <c r="G19" s="4" t="n">
-        <v>97.7</v>
+        <v>15</v>
       </c>
       <c r="H19" s="5" t="n">
         <v>300</v>
@@ -1586,7 +1726,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45876</v>
+        <v>45873</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
@@ -1600,12 +1740,12 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 9163456961</t>
+          <t>(E)429605</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>RAD64005012 -RADNOR™ 2" X 4 1/4"</t>
+          <t>tax</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
@@ -1614,7 +1754,7 @@
         </is>
       </c>
       <c r="G20" s="4" t="n">
-        <v>55</v>
+        <v>97.7</v>
       </c>
       <c r="H20" s="5" t="n">
         <v>300</v>
@@ -1641,7 +1781,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Indura®/Leather Flame Resistant Sleeves</t>
+          <t>RAD64005012 -RADNOR™ 2" X 4 1/4"</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
@@ -1650,7 +1790,7 @@
         </is>
       </c>
       <c r="G21" s="4" t="n">
-        <v>47.48</v>
+        <v>55</v>
       </c>
       <c r="H21" s="5" t="n">
         <v>300</v>
@@ -1677,7 +1817,7 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>tac</t>
+          <t>Indura®/Leather Flame Resistant Sleeves</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
@@ -1686,7 +1826,7 @@
         </is>
       </c>
       <c r="G22" s="4" t="n">
-        <v>7.94</v>
+        <v>47.48</v>
       </c>
       <c r="H22" s="5" t="n">
         <v>300</v>
@@ -1708,12 +1848,12 @@
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>9163809252</t>
+          <t xml:space="preserve"> 9163456961</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>LINED010203 -1/8" X 14" E6010 Fleetweld®</t>
+          <t>tac</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
@@ -1722,7 +1862,7 @@
         </is>
       </c>
       <c r="G23" s="4" t="n">
-        <v>735</v>
+        <v>7.94</v>
       </c>
       <c r="H23" s="5" t="n">
         <v>300</v>
@@ -1749,7 +1889,7 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>HazmatCharge</t>
+          <t>LINED010203 -1/8" X 14" E6010 Fleetweld®</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
@@ -1758,7 +1898,7 @@
         </is>
       </c>
       <c r="G24" s="4" t="n">
-        <v>45</v>
+        <v>735</v>
       </c>
       <c r="H24" s="5" t="n">
         <v>300</v>
@@ -1785,7 +1925,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>tax</t>
+          <t>HazmatCharge</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
@@ -1794,7 +1934,7 @@
         </is>
       </c>
       <c r="G25" s="4" t="n">
-        <v>60.45</v>
+        <v>45</v>
       </c>
       <c r="H25" s="5" t="n">
         <v>300</v>
@@ -1802,7 +1942,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45880</v>
+        <v>45876</v>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
@@ -1816,12 +1956,12 @@
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>9163809259</t>
+          <t>9163809252</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>7/8" Aluminum Oxide Type 27 Depressed</t>
+          <t>tax</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
@@ -1830,7 +1970,7 @@
         </is>
       </c>
       <c r="G26" s="4" t="n">
-        <v>12.27</v>
+        <v>60.45</v>
       </c>
       <c r="H26" s="5" t="n">
         <v>300</v>
@@ -1857,7 +1997,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>7/8" Ceramic Alumina Type 1 Cut Off Wheel</t>
+          <t>7/8" Aluminum Oxide Type 27 Depressed</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
@@ -1866,7 +2006,7 @@
         </is>
       </c>
       <c r="G27" s="4" t="n">
-        <v>140.5</v>
+        <v>12.27</v>
       </c>
       <c r="H27" s="5" t="n">
         <v>300</v>
@@ -1893,7 +2033,7 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>Taxes &amp; Fees</t>
+          <t>7/8" Ceramic Alumina Type 1 Cut Off Wheel</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
@@ -1902,7 +2042,7 @@
         </is>
       </c>
       <c r="G28" s="4" t="n">
-        <v>64.2</v>
+        <v>140.5</v>
       </c>
       <c r="H28" s="5" t="n">
         <v>300</v>
@@ -1929,7 +2069,7 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>7/8" Aluminum Oxide Type 1 Cut Off Wheel</t>
+          <t>Taxes &amp; Fees</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
@@ -1938,7 +2078,7 @@
         </is>
       </c>
       <c r="G29" s="4" t="n">
-        <v>49.92</v>
+        <v>64.2</v>
       </c>
       <c r="H29" s="5" t="n">
         <v>300</v>
@@ -1946,7 +2086,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45888</v>
+        <v>45880</v>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
@@ -1960,12 +2100,12 @@
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>1020070</t>
+          <t>9163809259</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>5"SCH10 PIPE(5.563"X.134")</t>
+          <t>7/8" Aluminum Oxide Type 1 Cut Off Wheel</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
@@ -1974,7 +2114,7 @@
         </is>
       </c>
       <c r="G30" s="4" t="n">
-        <v>5488.64</v>
+        <v>49.92</v>
       </c>
       <c r="H30" s="5" t="n">
         <v>300</v>
@@ -2001,7 +2141,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>3"SCH 40 A500B/A53B NON-HYDRO</t>
+          <t>5"SCH10 PIPE(5.563"X.134")</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
@@ -2010,7 +2150,7 @@
         </is>
       </c>
       <c r="G31" s="4" t="n">
-        <v>6174</v>
+        <v>5488.64</v>
       </c>
       <c r="H31" s="5" t="n">
         <v>300</v>
@@ -2037,7 +2177,7 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>2"SCH 40 A500B/A53B NON-HYDRO</t>
+          <t>3"SCH 40 A500B/A53B NON-HYDRO</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
@@ -2046,7 +2186,7 @@
         </is>
       </c>
       <c r="G32" s="4" t="n">
-        <v>846.72</v>
+        <v>6174</v>
       </c>
       <c r="H32" s="5" t="n">
         <v>300</v>
@@ -2054,35 +2194,35 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45889</v>
+        <v>45888</v>
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>5107.1 · Travel - Car Rental</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>Credit Card Charge</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>1020070</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>San Jose 8/19 - 8/20</t>
+          <t>2"SCH 40 A500B/A53B NON-HYDRO</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>2321 · Commerce Bank - Enterprise Acct</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G33" s="4" t="n">
-        <v>138.81</v>
+        <v>846.72</v>
       </c>
       <c r="H33" s="5" t="n">
         <v>300</v>
@@ -2090,35 +2230,35 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45891</v>
+        <v>45889</v>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5107.1 · Travel - Car Rental</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Credit Card Charge</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>16758</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>Gordon Doull Per diem for week of 8/25/2025 - 8/31/2025</t>
+          <t>San Jose 8/19 - 8/20</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2321 · Commerce Bank - Enterprise Acct</t>
         </is>
       </c>
       <c r="G34" s="4" t="n">
-        <v>100</v>
+        <v>138.81</v>
       </c>
       <c r="H34" s="5" t="n">
         <v>300</v>
@@ -2126,35 +2266,35 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45894</v>
+        <v>45891</v>
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>General Journal</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>(E)430000</t>
+          <t>16758</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>5 STD WELD CAP</t>
+          <t>Gordon Doull Per diem for week of 8/25/2025 - 8/31/2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
       <c r="G35" s="4" t="n">
-        <v>149.53</v>
+        <v>100</v>
       </c>
       <c r="H35" s="5" t="n">
         <v>300</v>
@@ -2181,7 +2321,7 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>3 STD WELD CAP</t>
+          <t>5 STD WELD CAP</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
@@ -2190,7 +2330,7 @@
         </is>
       </c>
       <c r="G36" s="4" t="n">
-        <v>16.98</v>
+        <v>149.53</v>
       </c>
       <c r="H36" s="5" t="n">
         <v>300</v>
@@ -2217,7 +2357,7 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>1 1/4 STD WELD CAP</t>
+          <t>3 STD WELD CAP</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
@@ -2226,7 +2366,7 @@
         </is>
       </c>
       <c r="G37" s="4" t="n">
-        <v>67.06999999999999</v>
+        <v>16.98</v>
       </c>
       <c r="H37" s="5" t="n">
         <v>300</v>
@@ -2253,7 +2393,7 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>2 X 6 BLK S-40 NIPPLE</t>
+          <t>1 1/4 STD WELD CAP</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
@@ -2262,7 +2402,7 @@
         </is>
       </c>
       <c r="G38" s="4" t="n">
-        <v>147.53</v>
+        <v>67.06999999999999</v>
       </c>
       <c r="H38" s="5" t="n">
         <v>300</v>
@@ -2289,7 +2429,7 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>3 X 6 BLK S-40 NIPPLE</t>
+          <t>2 X 6 BLK S-40 NIPPLE</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
@@ -2298,7 +2438,7 @@
         </is>
       </c>
       <c r="G39" s="4" t="n">
-        <v>286.88</v>
+        <v>147.53</v>
       </c>
       <c r="H39" s="5" t="n">
         <v>300</v>
@@ -2325,7 +2465,7 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>TAx</t>
+          <t>3 X 6 BLK S-40 NIPPLE</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
@@ -2334,7 +2474,7 @@
         </is>
       </c>
       <c r="G40" s="4" t="n">
-        <v>51.77</v>
+        <v>286.88</v>
       </c>
       <c r="H40" s="5" t="n">
         <v>300</v>
@@ -2346,7 +2486,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>5121 · Freight &amp; Shipping (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -2361,7 +2501,7 @@
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>Freight</t>
+          <t>TAx</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
@@ -2370,7 +2510,7 @@
         </is>
       </c>
       <c r="G41" s="4" t="n">
-        <v>15</v>
+        <v>51.77</v>
       </c>
       <c r="H41" s="5" t="n">
         <v>300</v>
@@ -2378,7 +2518,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45895</v>
+        <v>45894</v>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
@@ -2392,12 +2532,12 @@
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>2931578</t>
+          <t>(E)430000</t>
         </is>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>NY to San Jose</t>
+          <t>Freight</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
@@ -2406,7 +2546,7 @@
         </is>
       </c>
       <c r="G42" s="4" t="n">
-        <v>2750</v>
+        <v>15</v>
       </c>
       <c r="H42" s="5" t="n">
         <v>300</v>
@@ -2414,11 +2554,11 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45902</v>
+        <v>45895</v>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -2428,12 +2568,12 @@
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>1020430</t>
+          <t>2931578</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>5"SCH10 PIPE</t>
+          <t>NY to San Jose</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
@@ -2442,7 +2582,7 @@
         </is>
       </c>
       <c r="G43" s="4" t="n">
-        <v>3124.8</v>
+        <v>2750</v>
       </c>
       <c r="H43" s="5" t="n">
         <v>300</v>
@@ -2450,11 +2590,11 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45904</v>
+        <v>45902</v>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>5115 · Rent - Equipment (direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -2464,12 +2604,12 @@
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>252549305-001</t>
+          <t>1020430</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>375/0525 FENCE MODULAR 12' L X 6' H TEMPORARY PAN</t>
+          <t>5"SCH10 PIPE</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
@@ -2478,7 +2618,7 @@
         </is>
       </c>
       <c r="G44" s="4" t="n">
-        <v>58.1</v>
+        <v>3124.8</v>
       </c>
       <c r="H44" s="5" t="n">
         <v>300</v>
@@ -2505,7 +2645,7 @@
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>Delivery &amp; Pick up charge</t>
+          <t>375/0525 FENCE MODULAR 12' L X 6' H TEMPORARY PAN</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
@@ -2514,7 +2654,7 @@
         </is>
       </c>
       <c r="G45" s="4" t="n">
-        <v>370</v>
+        <v>58.1</v>
       </c>
       <c r="H45" s="5" t="n">
         <v>300</v>
@@ -2541,7 +2681,7 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>Service Charge and Tax</t>
+          <t>Delivery &amp; Pick up charge</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
@@ -2550,7 +2690,7 @@
         </is>
       </c>
       <c r="G46" s="4" t="n">
-        <v>108.6</v>
+        <v>370</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>300</v>
@@ -2577,7 +2717,7 @@
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>50 FENCE COVER</t>
+          <t>Service Charge and Tax</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
@@ -2586,7 +2726,7 @@
         </is>
       </c>
       <c r="G47" s="4" t="n">
-        <v>150</v>
+        <v>108.6</v>
       </c>
       <c r="H47" s="5" t="n">
         <v>300</v>
@@ -2594,11 +2734,11 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45909</v>
+        <v>45904</v>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -2608,12 +2748,12 @@
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>9164700138</t>
+          <t>252549305-001</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>7/8" Ceramic Alumina Type 1 Cut Off Wheel</t>
+          <t>50 FENCE COVER</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
@@ -2622,7 +2762,7 @@
         </is>
       </c>
       <c r="G48" s="4" t="n">
-        <v>219.18</v>
+        <v>150</v>
       </c>
       <c r="H48" s="5" t="n">
         <v>300</v>
@@ -2649,7 +2789,7 @@
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 7/8" Aluminum Oxide Type 1 Cut Off Wheel</t>
+          <t>7/8" Ceramic Alumina Type 1 Cut Off Wheel</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
@@ -2658,7 +2798,7 @@
         </is>
       </c>
       <c r="G49" s="4" t="n">
-        <v>142.08</v>
+        <v>219.18</v>
       </c>
       <c r="H49" s="5" t="n">
         <v>300</v>
@@ -2685,7 +2825,7 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>Single Sided Cotton Welder's Cap</t>
+          <t xml:space="preserve"> 7/8" Aluminum Oxide Type 1 Cut Off Wheel</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
@@ -2694,7 +2834,7 @@
         </is>
       </c>
       <c r="G50" s="4" t="n">
-        <v>15.36</v>
+        <v>142.08</v>
       </c>
       <c r="H50" s="5" t="n">
         <v>300</v>
@@ -2721,7 +2861,7 @@
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>Brown Top Grain Goatskin And Split Cowhide</t>
+          <t>Single Sided Cotton Welder's Cap</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
@@ -2730,7 +2870,7 @@
         </is>
       </c>
       <c r="G51" s="4" t="n">
-        <v>109.92</v>
+        <v>15.36</v>
       </c>
       <c r="H51" s="5" t="n">
         <v>300</v>
@@ -2757,7 +2897,7 @@
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>Tax &amp; HazMat Charge</t>
+          <t>Brown Top Grain Goatskin And Split Cowhide</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
@@ -2766,7 +2906,7 @@
         </is>
       </c>
       <c r="G52" s="4" t="n">
-        <v>94.47</v>
+        <v>109.92</v>
       </c>
       <c r="H52" s="5" t="n">
         <v>300</v>
@@ -2793,7 +2933,7 @@
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>7/8" Aluminum Oxide Type 27 Depressed</t>
+          <t>Tax &amp; HazMat Charge</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
@@ -2802,7 +2942,7 @@
         </is>
       </c>
       <c r="G53" s="4" t="n">
-        <v>61.35</v>
+        <v>94.47</v>
       </c>
       <c r="H53" s="5" t="n">
         <v>300</v>
@@ -2810,11 +2950,11 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45912</v>
+        <v>45909</v>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>5006 · Drilling Expense</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -2824,17 +2964,21 @@
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>738955</t>
-        </is>
-      </c>
-      <c r="E54" s="3" t="inlineStr"/>
+          <t>9164700138</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>7/8" Aluminum Oxide Type 27 Depressed</t>
+        </is>
+      </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
           <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G54" s="4" t="n">
-        <v>14115</v>
+        <v>61.35</v>
       </c>
       <c r="H54" s="5" t="n">
         <v>300</v>
@@ -2842,35 +2986,35 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45912</v>
+        <v>45910</v>
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>5107 · Travel - Other (Direct)</t>
+          <t>5107.1 · Travel - Car Rental</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Check</t>
+          <t>Credit Card Charge</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
         <is>
-          <t>EE_091225</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>uber to and from airport</t>
+          <t>Hoa Ma San Jose</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>1006.1 · (NEW) Calif B &amp; T Checking</t>
+          <t>2321 · Commerce Bank - Enterprise Acct</t>
         </is>
       </c>
       <c r="G55" s="4" t="n">
-        <v>110.94</v>
+        <v>236.86</v>
       </c>
       <c r="H55" s="5" t="n">
         <v>300</v>
@@ -2878,35 +3022,31 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45915</v>
+        <v>45912</v>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5006 · Drilling Expense</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>16767</t>
-        </is>
-      </c>
-      <c r="E56" s="3" t="inlineStr">
-        <is>
-          <t>Eric Ma Per diem for week of 9/15/2025 - 9/21/2025</t>
-        </is>
-      </c>
+          <t>738955</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr"/>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G56" s="4" t="n">
-        <v>150</v>
+        <v>14115</v>
       </c>
       <c r="H56" s="5" t="n">
         <v>300</v>
@@ -2914,35 +3054,35 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45915</v>
+        <v>45912</v>
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5107 · Travel - Other (Direct)</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Check</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
         <is>
-          <t>16767</t>
+          <t>EE_091225</t>
         </is>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>Gordon Doull Per diem for week of 9/15/2025 - 9/21/2025</t>
+          <t>uber to and from airport</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>1006.1 · (NEW) Calif B &amp; T Checking</t>
         </is>
       </c>
       <c r="G57" s="4" t="n">
-        <v>150</v>
+        <v>110.94</v>
       </c>
       <c r="H57" s="5" t="n">
         <v>300</v>
@@ -2969,7 +3109,7 @@
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>Iain Cowie Per diem for week of 9/15/2025 - 9/21/2025</t>
+          <t>Eric Ma Per diem for week of 9/15/2025 - 9/21/2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
@@ -2986,7 +3126,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45922</v>
+        <v>45915</v>
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
@@ -3000,12 +3140,12 @@
       </c>
       <c r="D59" s="3" t="inlineStr">
         <is>
-          <t>16768</t>
+          <t>16767</t>
         </is>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>Levi Winslow Per diem for week of 9/22/2025 - 9/28/2025</t>
+          <t>Gordon Doull Per diem for week of 9/15/2025 - 9/21/2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
@@ -3014,46 +3154,46 @@
         </is>
       </c>
       <c r="G59" s="4" t="n">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="H59" s="5" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45922</v>
+        <v>45915</v>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>5115 · Rent - Equipment (direct)</t>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>General Journal</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
         <is>
-          <t>174547431-0001</t>
+          <t>16767</t>
         </is>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>DLPKSRCHG</t>
+          <t>Iain Cowie Per diem for week of 9/15/2025 - 9/21/2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
       <c r="G60" s="4" t="n">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="H60" s="5" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="61">
@@ -3062,31 +3202,31 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>5115 · Rent - Equipment (direct)</t>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>General Journal</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
         <is>
-          <t>174547431-0001</t>
+          <t>16768</t>
         </is>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>Delivery &amp; Pick Up Charge</t>
+          <t>Levi Winslow Per diem for week of 9/22/2025 - 9/28/2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
       <c r="G61" s="4" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="H61" s="5" t="n">
         <v>400</v>
@@ -3111,14 +3251,18 @@
           <t>174547431-0001</t>
         </is>
       </c>
-      <c r="E62" s="3" t="inlineStr"/>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>DLPKSRCHG</t>
+        </is>
+      </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
           <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G62" s="4" t="n">
-        <v>25.5</v>
+        <v>72</v>
       </c>
       <c r="H62" s="5" t="n">
         <v>400</v>
@@ -3130,7 +3274,7 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>5121 · Freight &amp; Shipping (Direct)</t>
+          <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
@@ -3140,12 +3284,12 @@
       </c>
       <c r="D63" s="3" t="inlineStr">
         <is>
-          <t>2962520</t>
+          <t>174547431-0001</t>
         </is>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>NY to San Jose</t>
+          <t>Delivery &amp; Pick Up Charge</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
@@ -3154,7 +3298,7 @@
         </is>
       </c>
       <c r="G63" s="4" t="n">
-        <v>1450</v>
+        <v>400</v>
       </c>
       <c r="H63" s="5" t="n">
         <v>400</v>
@@ -3162,11 +3306,11 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45923</v>
+        <v>45922</v>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>5006 · Drilling Expense</t>
+          <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -3176,21 +3320,17 @@
       </c>
       <c r="D64" s="3" t="inlineStr">
         <is>
-          <t>SI-11HPU007130</t>
-        </is>
-      </c>
-      <c r="E64" s="3" t="inlineStr">
-        <is>
-          <t>CAP,PULL 1.25“ GP RODS</t>
-        </is>
-      </c>
+          <t>174547431-0001</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="inlineStr"/>
       <c r="F64" s="3" t="inlineStr">
         <is>
           <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G64" s="4" t="n">
-        <v>50</v>
+        <v>25.5</v>
       </c>
       <c r="H64" s="5" t="n">
         <v>400</v>
@@ -3198,11 +3338,11 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45923</v>
+        <v>45922</v>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>5006 · Drilling Expense</t>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
@@ -3212,12 +3352,12 @@
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>SI-11HPU007130</t>
+          <t>2962520</t>
         </is>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>NY to San Jose</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
@@ -3226,7 +3366,7 @@
         </is>
       </c>
       <c r="G65" s="4" t="n">
-        <v>97.52</v>
+        <v>1450</v>
       </c>
       <c r="H65" s="5" t="n">
         <v>400</v>
@@ -3238,7 +3378,7 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>5116 · Rent - Storage (Direct)</t>
+          <t>5006 · Drilling Expense</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -3253,7 +3393,7 @@
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>ROD,PROBE 1.25“ X 5‘</t>
+          <t>CAP,PULL 1.25“ GP RODS</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
@@ -3262,7 +3402,7 @@
         </is>
       </c>
       <c r="G66" s="4" t="n">
-        <v>990</v>
+        <v>50</v>
       </c>
       <c r="H66" s="5" t="n">
         <v>400</v>
@@ -3270,7 +3410,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45924</v>
+        <v>45923</v>
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
@@ -3284,12 +3424,12 @@
       </c>
       <c r="D67" s="3" t="inlineStr">
         <is>
-          <t>SI-11HPU007155</t>
+          <t>SI-11HPU007130</t>
         </is>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>PLUG,AUGER 6 1/4 3ª THICK  WOOD</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
@@ -3298,7 +3438,7 @@
         </is>
       </c>
       <c r="G67" s="4" t="n">
-        <v>640</v>
+        <v>97.52</v>
       </c>
       <c r="H67" s="5" t="n">
         <v>400</v>
@@ -3306,11 +3446,11 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45924</v>
+        <v>45923</v>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>5006 · Drilling Expense</t>
+          <t>5116 · Rent - Storage (Direct)</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
@@ -3320,12 +3460,12 @@
       </c>
       <c r="D68" s="3" t="inlineStr">
         <is>
-          <t>SI-11HPU007155</t>
+          <t>SI-11HPU007130</t>
         </is>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>PLUG,AUGER 4 1/4 THICK WOOD-CAS</t>
+          <t>ROD,PROBE 1.25“ X 5‘</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
@@ -3334,7 +3474,7 @@
         </is>
       </c>
       <c r="G68" s="4" t="n">
-        <v>332.5</v>
+        <v>990</v>
       </c>
       <c r="H68" s="5" t="n">
         <v>400</v>
@@ -3361,7 +3501,7 @@
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>BOLT,AUGER 2KEY 3 1/4 - 8 1/4 HD &amp; 4 1/4 - 7 1/4 XHD</t>
+          <t>PLUG,AUGER 6 1/4 3ª THICK  WOOD</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
@@ -3370,7 +3510,7 @@
         </is>
       </c>
       <c r="G69" s="4" t="n">
-        <v>200</v>
+        <v>640</v>
       </c>
       <c r="H69" s="5" t="n">
         <v>400</v>
@@ -3397,7 +3537,7 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>UPIN,1 5/8 HEX (5/8X2 3/8 STD)</t>
+          <t>PLUG,AUGER 4 1/4 THICK WOOD-CAS</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
@@ -3406,7 +3546,7 @@
         </is>
       </c>
       <c r="G70" s="4" t="n">
-        <v>34.98</v>
+        <v>332.5</v>
       </c>
       <c r="H70" s="5" t="n">
         <v>400</v>
@@ -3433,7 +3573,7 @@
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>TEETH,5T FORGED</t>
+          <t>BOLT,AUGER 2KEY 3 1/4 - 8 1/4 HD &amp; 4 1/4 - 7 1/4 XHD</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
@@ -3442,7 +3582,7 @@
         </is>
       </c>
       <c r="G71" s="4" t="n">
-        <v>1050</v>
+        <v>200</v>
       </c>
       <c r="H71" s="5" t="n">
         <v>400</v>
@@ -3469,7 +3609,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>HEAD,HSA 6 1/4 2KEY BULLET HD</t>
+          <t>UPIN,1 5/8 HEX (5/8X2 3/8 STD)</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
@@ -3478,7 +3618,7 @@
         </is>
       </c>
       <c r="G72" s="4" t="n">
-        <v>937.51</v>
+        <v>34.98</v>
       </c>
       <c r="H72" s="5" t="n">
         <v>400</v>
@@ -3505,7 +3645,7 @@
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>HEAD,HSA 8 1/4 2KEY BULLET HD</t>
+          <t>TEETH,5T FORGED</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
@@ -3514,7 +3654,7 @@
         </is>
       </c>
       <c r="G73" s="4" t="n">
-        <v>1400</v>
+        <v>1050</v>
       </c>
       <c r="H73" s="5" t="n">
         <v>400</v>
@@ -3541,7 +3681,7 @@
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>HSA,8 1/4 2KEY HD 5FT</t>
+          <t>HEAD,HSA 6 1/4 2KEY BULLET HD</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
@@ -3550,7 +3690,7 @@
         </is>
       </c>
       <c r="G74" s="4" t="n">
-        <v>3960</v>
+        <v>937.51</v>
       </c>
       <c r="H74" s="5" t="n">
         <v>400</v>
@@ -3577,7 +3717,7 @@
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>CETCO PUREGOLD MED CHIPS 50LB LOV</t>
+          <t>HEAD,HSA 8 1/4 2KEY BULLET HD</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
@@ -3586,7 +3726,7 @@
         </is>
       </c>
       <c r="G75" s="4" t="n">
-        <v>266.75</v>
+        <v>1400</v>
       </c>
       <c r="H75" s="5" t="n">
         <v>400</v>
@@ -3613,7 +3753,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>Delivery</t>
+          <t>HSA,8 1/4 2KEY HD 5FT</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
@@ -3622,7 +3762,7 @@
         </is>
       </c>
       <c r="G76" s="4" t="n">
-        <v>480</v>
+        <v>3960</v>
       </c>
       <c r="H76" s="5" t="n">
         <v>400</v>
@@ -3649,7 +3789,7 @@
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>CETCO PUREGOLD MED CHIPS 50LB LOV</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
@@ -3658,7 +3798,7 @@
         </is>
       </c>
       <c r="G77" s="4" t="n">
-        <v>872.0700000000001</v>
+        <v>266.75</v>
       </c>
       <c r="H77" s="5" t="n">
         <v>400</v>
@@ -3675,17 +3815,17 @@
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Credit</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
         <is>
-          <t>CM-11HPU000099</t>
+          <t>SI-11HPU007155</t>
         </is>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>HEAD,HSA 8 1/4 2KEY BULLET HD</t>
+          <t>Delivery</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
@@ -3694,7 +3834,7 @@
         </is>
       </c>
       <c r="G78" s="4" t="n">
-        <v>-1400</v>
+        <v>480</v>
       </c>
       <c r="H78" s="5" t="n">
         <v>400</v>
@@ -3711,17 +3851,17 @@
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Credit</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
         <is>
-          <t>CM-11HPU000099</t>
+          <t>SI-11HPU007155</t>
         </is>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>HSA,8 1/4 2KEY HD 5FT</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
@@ -3730,7 +3870,7 @@
         </is>
       </c>
       <c r="G79" s="4" t="n">
-        <v>-3960</v>
+        <v>872.0700000000001</v>
       </c>
       <c r="H79" s="5" t="n">
         <v>400</v>
@@ -3757,7 +3897,7 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>HEAD,HSA 8 1/4 2KEY BULLET HD</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
@@ -3766,7 +3906,7 @@
         </is>
       </c>
       <c r="G80" s="4" t="n">
-        <v>-502.5</v>
+        <v>-1400</v>
       </c>
       <c r="H80" s="5" t="n">
         <v>400</v>
@@ -3793,7 +3933,7 @@
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>HEAD,HSA 8 1/4 2KEY BULLET HD</t>
+          <t>HSA,8 1/4 2KEY HD 5FT</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
@@ -3802,7 +3942,7 @@
         </is>
       </c>
       <c r="G81" s="4" t="n">
-        <v>1400</v>
+        <v>-3960</v>
       </c>
       <c r="H81" s="5" t="n">
         <v>400</v>
@@ -3829,7 +3969,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>HSA,8 1/4 2KEY HD 5FT</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
@@ -3838,7 +3978,7 @@
         </is>
       </c>
       <c r="G82" s="4" t="n">
-        <v>3960</v>
+        <v>-502.5</v>
       </c>
       <c r="H82" s="5" t="n">
         <v>400</v>
@@ -3865,7 +4005,7 @@
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>HEAD,HSA 8 1/4 2KEY BULLET HD</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
@@ -3874,7 +4014,7 @@
         </is>
       </c>
       <c r="G83" s="4" t="n">
-        <v>502.5</v>
+        <v>1400</v>
       </c>
       <c r="H83" s="5" t="n">
         <v>400</v>
@@ -3886,22 +4026,22 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5006 · Drilling Expense</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>Credit</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>SI-11HPU007154</t>
+          <t>CM-11HPU000099</t>
         </is>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>HEAD,HSA 4 1/4 2KEY BULLET HD(4 SM07 CUTTERS)</t>
+          <t>HSA,8 1/4 2KEY HD 5FT</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
@@ -3910,7 +4050,7 @@
         </is>
       </c>
       <c r="G84" s="4" t="n">
-        <v>500</v>
+        <v>3960</v>
       </c>
       <c r="H84" s="5" t="n">
         <v>400</v>
@@ -3922,22 +4062,22 @@
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5006 · Drilling Expense</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>Credit</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>SI-11HPU007154</t>
+          <t>CM-11HPU000099</t>
         </is>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>HSA,6 1/4 2 KEY HD X 5FT</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
@@ -3946,7 +4086,7 @@
         </is>
       </c>
       <c r="G85" s="4" t="n">
-        <v>1880</v>
+        <v>502.5</v>
       </c>
       <c r="H85" s="5" t="n">
         <v>400</v>
@@ -3973,7 +4113,7 @@
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>HEAD,HSA 4 1/4 2KEY BULLET HD(4 SM07 CUTTERS)</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
@@ -3982,7 +4122,7 @@
         </is>
       </c>
       <c r="G86" s="4" t="n">
-        <v>223.13</v>
+        <v>500</v>
       </c>
       <c r="H86" s="5" t="n">
         <v>400</v>
@@ -3990,35 +4130,35 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45929</v>
+        <v>45924</v>
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>16772</t>
+          <t>SI-11HPU007154</t>
         </is>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>Levi Winslow Per diem for week of 9/29/2025 - 10/5/2025</t>
+          <t>HSA,6 1/4 2 KEY HD X 5FT</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G87" s="4" t="n">
-        <v>350</v>
+        <v>1880</v>
       </c>
       <c r="H87" s="5" t="n">
         <v>400</v>
@@ -4026,35 +4166,35 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>45929</v>
+        <v>45924</v>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>16772</t>
+          <t>SI-11HPU007154</t>
         </is>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>Luke Giguere Per diem for week of 9/29/2025 - 10/5/2025</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G88" s="4" t="n">
-        <v>350</v>
+        <v>223.13</v>
       </c>
       <c r="H88" s="5" t="n">
         <v>400</v>
@@ -4062,181 +4202,1537 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>45929</v>
+        <v>45924</v>
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5123 · Auto fuel (Direct)</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Credit Card Charge</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>16772</t>
-        </is>
-      </c>
-      <c r="E89" s="3" t="inlineStr">
-        <is>
-          <t>Michael Hyatt Per diem for week of 9/29/2025 - 10/5/2025</t>
-        </is>
-      </c>
+          <t>BV</t>
+        </is>
+      </c>
+      <c r="E89" s="3" t="inlineStr"/>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2323 · Shell Credit Card - WEX</t>
         </is>
       </c>
       <c r="G89" s="4" t="n">
-        <v>350</v>
+        <v>105.27</v>
       </c>
       <c r="H89" s="5" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>45929</v>
+        <v>45925</v>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
         <is>
-          <t>16772</t>
+          <t>9655231844</t>
         </is>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>Mike Cogswell Per diem for week of 9/29/2025 - 10/5/2025</t>
+          <t>HOODED COVERALLS,XL,WHITE,BULK,PK25</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G90" s="4" t="n">
-        <v>350</v>
+        <v>65.2</v>
       </c>
       <c r="H90" s="5" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>45933</v>
+        <v>45925</v>
       </c>
       <c r="B91" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
         <is>
-          <t>16773</t>
+          <t>9655231844</t>
         </is>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>Brian Vives Per diem for week of 10/6/2025 - 10/12/2025</t>
+          <t>HOODED COVERALLS,L,WHITE,BULK,PK25</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G91" s="4" t="n">
-        <v>100</v>
+        <v>63.73</v>
       </c>
       <c r="H91" s="5" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>45933</v>
+        <v>45925</v>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
         <is>
-          <t>16773</t>
+          <t>9655231844</t>
         </is>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>Gordon Doull Per diem for week of 10/6/2025 - 10/12/2025</t>
+          <t>SPILL KIT</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G92" s="4" t="n">
-        <v>50</v>
+        <v>398.32</v>
       </c>
       <c r="H92" s="5" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
+        <v>45925</v>
+      </c>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="inlineStr">
+        <is>
+          <t>9655231844</t>
+        </is>
+      </c>
+      <c r="E93" s="3" t="inlineStr">
+        <is>
+          <t>ABSORB PAD,OIL-BASED LIQUIDS,WHITE,PK20</t>
+        </is>
+      </c>
+      <c r="F93" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G93" s="4" t="n">
+        <v>71.36</v>
+      </c>
+      <c r="H93" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>45925</v>
+      </c>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="inlineStr">
+        <is>
+          <t>9655231844</t>
+        </is>
+      </c>
+      <c r="E94" s="3" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F94" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G94" s="4" t="n">
+        <v>56.12</v>
+      </c>
+      <c r="H94" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>45925</v>
+      </c>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>5128 · Health &amp; Safety Equip (Direct)</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="inlineStr">
+        <is>
+          <t>9654451104</t>
+        </is>
+      </c>
+      <c r="E95" s="3" t="inlineStr">
+        <is>
+          <t>HALF MASK RESPIRATOR,ELASTOMER,BLACK</t>
+        </is>
+      </c>
+      <c r="F95" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G95" s="4" t="n">
+        <v>69.3</v>
+      </c>
+      <c r="H95" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>45925</v>
+      </c>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>5128 · Health &amp; Safety Equip (Direct)</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D96" s="3" t="inlineStr">
+        <is>
+          <t>9654451104</t>
+        </is>
+      </c>
+      <c r="E96" s="3" t="inlineStr">
+        <is>
+          <t>COMBINATION CARTRIDGE/FILTER,THREADED,PR</t>
+        </is>
+      </c>
+      <c r="F96" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G96" s="4" t="n">
+        <v>196.74</v>
+      </c>
+      <c r="H96" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45925</v>
+      </c>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>5128 · Health &amp; Safety Equip (Direct)</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="inlineStr">
+        <is>
+          <t>9654451104</t>
+        </is>
+      </c>
+      <c r="E97" s="3" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F97" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G97" s="4" t="n">
+        <v>24.94</v>
+      </c>
+      <c r="H97" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>45928</v>
+      </c>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>5123 · Auto fuel (Direct)</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="inlineStr">
+        <is>
+          <t>Credit Card Charge</t>
+        </is>
+      </c>
+      <c r="D98" s="3" t="inlineStr">
+        <is>
+          <t>BV</t>
+        </is>
+      </c>
+      <c r="E98" s="3" t="inlineStr"/>
+      <c r="F98" s="3" t="inlineStr">
+        <is>
+          <t>2323 · Shell Credit Card - WEX</t>
+        </is>
+      </c>
+      <c r="G98" s="4" t="n">
+        <v>119.53</v>
+      </c>
+      <c r="H98" s="5" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D99" s="3" t="inlineStr">
+        <is>
+          <t>16772</t>
+        </is>
+      </c>
+      <c r="E99" s="3" t="inlineStr">
+        <is>
+          <t>Levi Winslow Per diem for week of 9/29/2025 - 10/5/2025</t>
+        </is>
+      </c>
+      <c r="F99" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G99" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H99" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B100" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C100" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D100" s="3" t="inlineStr">
+        <is>
+          <t>16772</t>
+        </is>
+      </c>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>Luke Giguere Per diem for week of 9/29/2025 - 10/5/2025</t>
+        </is>
+      </c>
+      <c r="F100" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G100" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H100" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B101" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C101" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>16772</t>
+        </is>
+      </c>
+      <c r="E101" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt Per diem for week of 9/29/2025 - 10/5/2025</t>
+        </is>
+      </c>
+      <c r="F101" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G101" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H101" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B102" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C102" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D102" s="3" t="inlineStr">
+        <is>
+          <t>16772</t>
+        </is>
+      </c>
+      <c r="E102" s="3" t="inlineStr">
+        <is>
+          <t>Mike Cogswell Per diem for week of 9/29/2025 - 10/5/2025</t>
+        </is>
+      </c>
+      <c r="F102" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G102" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H102" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C103" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D103" s="3" t="inlineStr">
+        <is>
+          <t>SI-11HPU007182</t>
+        </is>
+      </c>
+      <c r="E103" s="3" t="inlineStr">
+        <is>
+          <t>SAND,#3 50LB KLEEN LAPIS GOLD</t>
+        </is>
+      </c>
+      <c r="F103" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G103" s="4" t="n">
+        <v>5409.6</v>
+      </c>
+      <c r="H103" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D104" s="3" t="inlineStr">
+        <is>
+          <t>SI-11HPU007182</t>
+        </is>
+      </c>
+      <c r="E104" s="3" t="inlineStr">
+        <is>
+          <t>CETCO PUREGOLD MED CHIPS 50LB LOV</t>
+        </is>
+      </c>
+      <c r="F104" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G104" s="4" t="n">
+        <v>512.16</v>
+      </c>
+      <c r="H104" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D105" s="3" t="inlineStr">
+        <is>
+          <t>SI-11HPU007182</t>
+        </is>
+      </c>
+      <c r="E105" s="3" t="inlineStr">
+        <is>
+          <t>CAP,DRIVE AUGER 4 1/4 2KEY HD 1 5/8 HEX</t>
+        </is>
+      </c>
+      <c r="F105" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G105" s="4" t="n">
+        <v>450</v>
+      </c>
+      <c r="H105" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B106" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D106" s="3" t="inlineStr">
+        <is>
+          <t>SI-11HPU007182</t>
+        </is>
+      </c>
+      <c r="E106" s="3" t="inlineStr">
+        <is>
+          <t>Delivery</t>
+        </is>
+      </c>
+      <c r="F106" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G106" s="4" t="n">
+        <v>250</v>
+      </c>
+      <c r="H106" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45929</v>
+      </c>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D107" s="3" t="inlineStr">
+        <is>
+          <t>SI-11HPU007182</t>
+        </is>
+      </c>
+      <c r="E107" s="3" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G107" s="4" t="n">
+        <v>620.8099999999999</v>
+      </c>
+      <c r="H107" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B108" s="3" t="inlineStr">
+        <is>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="inlineStr">
+        <is>
+          <t>Invoice</t>
+        </is>
+      </c>
+      <c r="D108" s="3" t="inlineStr">
+        <is>
+          <t>NGSJ25-003</t>
+        </is>
+      </c>
+      <c r="E108" s="3" t="inlineStr">
+        <is>
+          <t>Load &amp; Ship to Site</t>
+        </is>
+      </c>
+      <c r="F108" s="3" t="inlineStr">
+        <is>
+          <t>1100 · Trade Debtors</t>
+        </is>
+      </c>
+      <c r="G108" s="4" t="n">
+        <v>13000</v>
+      </c>
+      <c r="H108" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B109" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C109" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D109" s="3" t="inlineStr">
+        <is>
+          <t>252549305-002</t>
+        </is>
+      </c>
+      <c r="E109" s="3" t="inlineStr">
+        <is>
+          <t>375/0525 FENCE MODULAR 12' L X 6' H TEMPORARY PAN</t>
+        </is>
+      </c>
+      <c r="F109" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G109" s="4" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="H109" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B110" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C110" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D110" s="3" t="inlineStr">
+        <is>
+          <t>252549305-002</t>
+        </is>
+      </c>
+      <c r="E110" s="3" t="inlineStr">
+        <is>
+          <t>Fence Wheel and weight</t>
+        </is>
+      </c>
+      <c r="F110" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G110" s="4" t="n">
+        <v>65</v>
+      </c>
+      <c r="H110" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B111" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C111" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D111" s="3" t="inlineStr">
+        <is>
+          <t>252549305-002</t>
+        </is>
+      </c>
+      <c r="E111" s="3" t="inlineStr">
+        <is>
+          <t>Service Charge and Tax</t>
+        </is>
+      </c>
+      <c r="F111" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G111" s="4" t="n">
+        <v>11.61</v>
+      </c>
+      <c r="H111" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
         <v>45933</v>
       </c>
-      <c r="B93" s="3" t="inlineStr">
+      <c r="B112" s="3" t="inlineStr">
         <is>
           <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
-      <c r="C93" s="3" t="inlineStr">
+      <c r="C112" s="3" t="inlineStr">
         <is>
           <t>General Journal</t>
         </is>
       </c>
-      <c r="D93" s="3" t="inlineStr">
+      <c r="D112" s="3" t="inlineStr">
         <is>
           <t>16773</t>
         </is>
       </c>
-      <c r="E93" s="3" t="inlineStr">
+      <c r="E112" s="3" t="inlineStr">
+        <is>
+          <t>Brian Vives Per diem for week of 10/6/2025 - 10/12/2025</t>
+        </is>
+      </c>
+      <c r="F112" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G112" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H112" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B113" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C113" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D113" s="3" t="inlineStr">
+        <is>
+          <t>16773</t>
+        </is>
+      </c>
+      <c r="E113" s="3" t="inlineStr">
+        <is>
+          <t>Gordon Doull Per diem for week of 10/6/2025 - 10/12/2025</t>
+        </is>
+      </c>
+      <c r="F113" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G113" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="H113" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B114" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C114" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D114" s="3" t="inlineStr">
+        <is>
+          <t>16773</t>
+        </is>
+      </c>
+      <c r="E114" s="3" t="inlineStr">
         <is>
           <t>Michael Hyatt Per diem for week of 10/6/2025 - 10/12/2025</t>
         </is>
       </c>
-      <c r="F93" s="3" t="inlineStr">
+      <c r="F114" s="3" t="inlineStr">
         <is>
           <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
-      <c r="G93" s="4" t="n">
+      <c r="G114" s="4" t="n">
         <v>350</v>
       </c>
-      <c r="H93" s="5" t="n">
+      <c r="H114" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="B115" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C115" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D115" s="3" t="inlineStr">
+        <is>
+          <t>174547431-0002</t>
+        </is>
+      </c>
+      <c r="E115" s="3" t="inlineStr">
+        <is>
+          <t>DUCT JACK/MATERIAL 24'-26'</t>
+        </is>
+      </c>
+      <c r="F115" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G115" s="4" t="n">
+        <v>755</v>
+      </c>
+      <c r="H115" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="B116" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C116" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D116" s="3" t="inlineStr">
+        <is>
+          <t>174547431-0002</t>
+        </is>
+      </c>
+      <c r="E116" s="3" t="inlineStr">
+        <is>
+          <t>DSL TRACK MINI SKIDSTEER</t>
+        </is>
+      </c>
+      <c r="F116" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G116" s="4" t="n">
+        <v>2965</v>
+      </c>
+      <c r="H116" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="B117" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C117" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D117" s="3" t="inlineStr">
+        <is>
+          <t>174547431-0002</t>
+        </is>
+      </c>
+      <c r="E117" s="3" t="inlineStr">
+        <is>
+          <t>10K 42'-48' TELEHANDLER FORKLIFT</t>
+        </is>
+      </c>
+      <c r="F117" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G117" s="4" t="n">
+        <v>4695</v>
+      </c>
+      <c r="H117" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="B118" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C118" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D118" s="3" t="inlineStr">
+        <is>
+          <t>174547431-0002</t>
+        </is>
+      </c>
+      <c r="E118" s="3" t="inlineStr">
+        <is>
+          <t>Delivery &amp; PickUp</t>
+        </is>
+      </c>
+      <c r="F118" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G118" s="4" t="n">
+        <v>440</v>
+      </c>
+      <c r="H118" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>45938</v>
+      </c>
+      <c r="B119" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C119" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D119" s="3" t="inlineStr">
+        <is>
+          <t>174547431-0002</t>
+        </is>
+      </c>
+      <c r="E119" s="3" t="inlineStr">
+        <is>
+          <t>Fees &amp; tax</t>
+        </is>
+      </c>
+      <c r="F119" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G119" s="4" t="n">
+        <v>1041.93</v>
+      </c>
+      <c r="H119" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>45941</v>
+      </c>
+      <c r="B120" s="3" t="inlineStr">
+        <is>
+          <t>5006 · Drilling Expense</t>
+        </is>
+      </c>
+      <c r="C120" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D120" s="3" t="inlineStr">
+        <is>
+          <t>738975</t>
+        </is>
+      </c>
+      <c r="E120" s="3" t="inlineStr"/>
+      <c r="F120" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G120" s="4" t="n">
+        <v>1600</v>
+      </c>
+      <c r="H120" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="B121" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C121" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D121" s="3" t="inlineStr">
+        <is>
+          <t>16774</t>
+        </is>
+      </c>
+      <c r="E121" s="3" t="inlineStr">
+        <is>
+          <t>Mike Cogswell Per diem for week of 10/13/2025 - 10/19/2025</t>
+        </is>
+      </c>
+      <c r="F121" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G121" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H121" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="B122" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C122" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D122" s="3" t="inlineStr">
+        <is>
+          <t>16774</t>
+        </is>
+      </c>
+      <c r="E122" s="3" t="inlineStr">
+        <is>
+          <t>Shane Morris Per diem for week of 10/13/2025 - 10/19/2025</t>
+        </is>
+      </c>
+      <c r="F122" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G122" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H122" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="B123" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C123" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D123" s="3" t="inlineStr">
+        <is>
+          <t>16774</t>
+        </is>
+      </c>
+      <c r="E123" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh Per diem for week of 10/13/2025 - 10/19/2025</t>
+        </is>
+      </c>
+      <c r="F123" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G123" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H123" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45944</v>
+      </c>
+      <c r="B124" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C124" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D124" s="3" t="inlineStr">
+        <is>
+          <t>16774</t>
+        </is>
+      </c>
+      <c r="E124" s="3" t="inlineStr">
+        <is>
+          <t>Wyatt Staples Per diem for week of 10/13/2025 - 10/19/2025</t>
+        </is>
+      </c>
+      <c r="F124" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G124" s="4" t="n">
+        <v>300</v>
+      </c>
+      <c r="H124" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45947</v>
+      </c>
+      <c r="B125" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C125" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D125" s="3" t="inlineStr">
+        <is>
+          <t>16777</t>
+        </is>
+      </c>
+      <c r="E125" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt Per diem for week of 10/20/2025 - 10/26/2025</t>
+        </is>
+      </c>
+      <c r="F125" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G125" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H125" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>45947</v>
+      </c>
+      <c r="B126" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C126" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D126" s="3" t="inlineStr">
+        <is>
+          <t>16777</t>
+        </is>
+      </c>
+      <c r="E126" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh Per diem for week of 10/20/2025 - 10/26/2025</t>
+        </is>
+      </c>
+      <c r="F126" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G126" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H126" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>45951</v>
+      </c>
+      <c r="B127" s="3" t="inlineStr">
+        <is>
+          <t>1504 · Undeposited Funds</t>
+        </is>
+      </c>
+      <c r="C127" s="3" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="D127" s="3" t="inlineStr">
+        <is>
+          <t>35191</t>
+        </is>
+      </c>
+      <c r="E127" s="3" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="F127" s="3" t="inlineStr">
+        <is>
+          <t>1006.1 · (NEW) Calif B &amp; T Checking</t>
+        </is>
+      </c>
+      <c r="G127" s="4" t="n">
+        <v>45072</v>
+      </c>
+      <c r="H127" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="B128" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C128" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D128" s="3" t="inlineStr">
+        <is>
+          <t>16779</t>
+        </is>
+      </c>
+      <c r="E128" s="3" t="inlineStr">
+        <is>
+          <t>Brian Vives Per diem for week of 10/27/2025 - 11/02/2025</t>
+        </is>
+      </c>
+      <c r="F128" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G128" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H128" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="B129" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C129" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D129" s="3" t="inlineStr">
+        <is>
+          <t>16779</t>
+        </is>
+      </c>
+      <c r="E129" s="3" t="inlineStr">
+        <is>
+          <t>Gordon Doull Per diem for week of 10/27/2025 - 11/02/2025</t>
+        </is>
+      </c>
+      <c r="F129" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G129" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="H129" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="B130" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C130" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D130" s="3" t="inlineStr">
+        <is>
+          <t>16779</t>
+        </is>
+      </c>
+      <c r="E130" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt Per diem for week of 10/27/2025 - 11/02/2025</t>
+        </is>
+      </c>
+      <c r="F130" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G130" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H130" s="5" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="B131" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C131" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D131" s="3" t="inlineStr">
+        <is>
+          <t>16779</t>
+        </is>
+      </c>
+      <c r="E131" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh Per diem for week of 10/27/2025 - 11/02/2025</t>
+        </is>
+      </c>
+      <c r="F131" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G131" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H131" s="5" t="n">
         <v>400</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update web reports - 2026-02-20 21:00:54
</commit_message>
<xml_diff>
--- a/quickbook_summary.xlsx
+++ b/quickbook_summary.xlsx
@@ -3076,7 +3076,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>46053</v>
+        <v>46056</v>
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
@@ -3106,13 +3106,15 @@
       <c r="G73" s="4" t="n">
         <v>11407.5</v>
       </c>
-      <c r="H73" s="5" t="n">
-        <v>500</v>
+      <c r="H73" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>46053</v>
+        <v>46056</v>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
@@ -3142,13 +3144,15 @@
       <c r="G74" s="4" t="n">
         <v>54602.32</v>
       </c>
-      <c r="H74" s="5" t="n">
-        <v>500</v>
+      <c r="H74" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>46053</v>
+        <v>46056</v>
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
@@ -3178,13 +3182,15 @@
       <c r="G75" s="4" t="n">
         <v>50518</v>
       </c>
-      <c r="H75" s="5" t="n">
-        <v>500</v>
+      <c r="H75" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>46053</v>
+        <v>46056</v>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
@@ -3214,13 +3220,15 @@
       <c r="G76" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H76" s="5" t="n">
-        <v>500</v>
+      <c r="H76" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>46053</v>
+        <v>46056</v>
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
@@ -3250,13 +3258,15 @@
       <c r="G77" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H77" s="5" t="n">
-        <v>500</v>
+      <c r="H77" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>46053</v>
+        <v>46056</v>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
@@ -3286,8 +3296,10 @@
       <c r="G78" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H78" s="5" t="n">
-        <v>500</v>
+      <c r="H78" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -3301,7 +3313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H380"/>
+  <dimension ref="A1:H433"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -16334,74 +16346,78 @@
     </row>
     <row r="367">
       <c r="A367" s="2" t="n">
-        <v>46038</v>
+        <v>46036</v>
       </c>
       <c r="B367" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C367" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D367" s="3" t="inlineStr">
         <is>
-          <t>16810</t>
+          <t>9771267425</t>
         </is>
       </c>
       <c r="E367" s="3" t="inlineStr">
         <is>
-          <t>Luke Giguere Per diem for week of 1/19/2026 - 1/25/2026</t>
+          <t>THREE BEAM MAGNETIC TORPEDO LASER LEVEL</t>
         </is>
       </c>
       <c r="F367" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G367" s="4" t="n">
-        <v>350</v>
-      </c>
-      <c r="H367" s="5" t="n">
-        <v>500</v>
+        <v>189.76</v>
+      </c>
+      <c r="H367" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="2" t="n">
-        <v>46038</v>
+        <v>46036</v>
       </c>
       <c r="B368" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C368" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D368" s="3" t="inlineStr">
         <is>
-          <t>16810</t>
+          <t>9771267425</t>
         </is>
       </c>
       <c r="E368" s="3" t="inlineStr">
         <is>
-          <t>Michael Hyatt Per diem for week of 1/12/2026 - 1/25/2026</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F368" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G368" s="4" t="n">
-        <v>700</v>
-      </c>
-      <c r="H368" s="5" t="n">
-        <v>500</v>
+        <v>14.71</v>
+      </c>
+      <c r="H368" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="369">
@@ -16410,31 +16426,31 @@
       </c>
       <c r="B369" s="3" t="inlineStr">
         <is>
-          <t>5115 · Rent - Equipment (direct)</t>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
       <c r="C369" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>General Journal</t>
         </is>
       </c>
       <c r="D369" s="3" t="inlineStr">
         <is>
-          <t>178433028-0001</t>
+          <t>16810</t>
         </is>
       </c>
       <c r="E369" s="3" t="inlineStr">
         <is>
-          <t>10K 42'-48' TELEHANDLER FORKLIFT</t>
+          <t>Luke Giguere Per diem for week of 1/19/2026 - 1/25/2026</t>
         </is>
       </c>
       <c r="F369" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
       <c r="G369" s="4" t="n">
-        <v>4470</v>
+        <v>350</v>
       </c>
       <c r="H369" s="5" t="n">
         <v>500</v>
@@ -16446,31 +16462,31 @@
       </c>
       <c r="B370" s="3" t="inlineStr">
         <is>
-          <t>5115 · Rent - Equipment (direct)</t>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
       <c r="C370" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>General Journal</t>
         </is>
       </c>
       <c r="D370" s="3" t="inlineStr">
         <is>
-          <t>178433028-0001</t>
+          <t>16810</t>
         </is>
       </c>
       <c r="E370" s="3" t="inlineStr">
         <is>
-          <t>Fees and Charges</t>
+          <t>Michael Hyatt Per diem for week of 1/12/2026 - 1/25/2026</t>
         </is>
       </c>
       <c r="F370" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
       <c r="G370" s="4" t="n">
-        <v>190.69</v>
+        <v>700</v>
       </c>
       <c r="H370" s="5" t="n">
         <v>500</v>
@@ -16497,7 +16513,7 @@
       </c>
       <c r="E371" s="3" t="inlineStr">
         <is>
-          <t>Delivery &amp; Pick Up Charge</t>
+          <t>10K 42'-48' TELEHANDLER FORKLIFT</t>
         </is>
       </c>
       <c r="F371" s="3" t="inlineStr">
@@ -16506,7 +16522,7 @@
         </is>
       </c>
       <c r="G371" s="4" t="n">
-        <v>400</v>
+        <v>4470</v>
       </c>
       <c r="H371" s="5" t="n">
         <v>500</v>
@@ -16533,7 +16549,7 @@
       </c>
       <c r="E372" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>Fees and Charges</t>
         </is>
       </c>
       <c r="F372" s="3" t="inlineStr">
@@ -16542,7 +16558,7 @@
         </is>
       </c>
       <c r="G372" s="4" t="n">
-        <v>455.68</v>
+        <v>190.69</v>
       </c>
       <c r="H372" s="5" t="n">
         <v>500</v>
@@ -16550,11 +16566,11 @@
     </row>
     <row r="373">
       <c r="A373" s="2" t="n">
-        <v>46041</v>
+        <v>46038</v>
       </c>
       <c r="B373" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
       <c r="C373" s="3" t="inlineStr">
@@ -16564,12 +16580,12 @@
       </c>
       <c r="D373" s="3" t="inlineStr">
         <is>
-          <t>58310926</t>
+          <t>178433028-0001</t>
         </is>
       </c>
       <c r="E373" s="3" t="inlineStr">
         <is>
-          <t>316 Stainless Steel Check Valve with Fluoroelastomer Piston with Rubber</t>
+          <t>Delivery &amp; Pick Up Charge</t>
         </is>
       </c>
       <c r="F373" s="3" t="inlineStr">
@@ -16578,7 +16594,7 @@
         </is>
       </c>
       <c r="G373" s="4" t="n">
-        <v>787.6799999999999</v>
+        <v>400</v>
       </c>
       <c r="H373" s="5" t="n">
         <v>500</v>
@@ -16586,11 +16602,11 @@
     </row>
     <row r="374">
       <c r="A374" s="2" t="n">
-        <v>46041</v>
+        <v>46038</v>
       </c>
       <c r="B374" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
       <c r="C374" s="3" t="inlineStr">
@@ -16600,7 +16616,7 @@
       </c>
       <c r="D374" s="3" t="inlineStr">
         <is>
-          <t>58310926</t>
+          <t>178433028-0001</t>
         </is>
       </c>
       <c r="E374" s="3" t="inlineStr">
@@ -16614,7 +16630,7 @@
         </is>
       </c>
       <c r="G374" s="4" t="n">
-        <v>43.32</v>
+        <v>455.68</v>
       </c>
       <c r="H374" s="5" t="n">
         <v>500</v>
@@ -16626,7 +16642,7 @@
       </c>
       <c r="B375" s="3" t="inlineStr">
         <is>
-          <t>5121 · Freight &amp; Shipping (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C375" s="3" t="inlineStr">
@@ -16641,7 +16657,7 @@
       </c>
       <c r="E375" s="3" t="inlineStr">
         <is>
-          <t>Shipping</t>
+          <t>316 Stainless Steel Check Valve with Fluoroelastomer Piston with Rubber</t>
         </is>
       </c>
       <c r="F375" s="3" t="inlineStr">
@@ -16650,7 +16666,7 @@
         </is>
       </c>
       <c r="G375" s="4" t="n">
-        <v>16.44</v>
+        <v>787.6799999999999</v>
       </c>
       <c r="H375" s="5" t="n">
         <v>500</v>
@@ -16658,35 +16674,35 @@
     </row>
     <row r="376">
       <c r="A376" s="2" t="n">
-        <v>46045</v>
+        <v>46041</v>
       </c>
       <c r="B376" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C376" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D376" s="3" t="inlineStr">
         <is>
-          <t>16811</t>
+          <t>58310926</t>
         </is>
       </c>
       <c r="E376" s="3" t="inlineStr">
         <is>
-          <t>Luke Giguere per diem Per diem for week of 1/26/2026 - 2/21/2026</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F376" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G376" s="4" t="n">
-        <v>350</v>
+        <v>43.32</v>
       </c>
       <c r="H376" s="5" t="n">
         <v>500</v>
@@ -16694,107 +16710,111 @@
     </row>
     <row r="377">
       <c r="A377" s="2" t="n">
-        <v>46045</v>
+        <v>46041</v>
       </c>
       <c r="B377" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C377" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D377" s="3" t="inlineStr">
         <is>
-          <t>16811</t>
+          <t>9775828545</t>
         </is>
       </c>
       <c r="E377" s="3" t="inlineStr">
         <is>
-          <t>Michael Hyatt per diem Per diem for week of 1/26/2026 - 2/21/2026</t>
+          <t>V-BELT PULLEY,DETACHABLE,3GROOVE,7.75"O</t>
         </is>
       </c>
       <c r="F377" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G377" s="4" t="n">
-        <v>350</v>
-      </c>
-      <c r="H377" s="5" t="n">
-        <v>500</v>
+        <v>222.11</v>
+      </c>
+      <c r="H377" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="2" t="n">
-        <v>46045</v>
+        <v>46041</v>
       </c>
       <c r="B378" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C378" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D378" s="3" t="inlineStr">
         <is>
-          <t>16811</t>
+          <t>9775828545</t>
         </is>
       </c>
       <c r="E378" s="3" t="inlineStr">
         <is>
-          <t>Michael Hyatt per diem Per diem for week of 1/17/2026 - 1/18/2026</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="F378" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G378" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="H378" s="5" t="n">
-        <v>500</v>
+        <v>17.22</v>
+      </c>
+      <c r="H378" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="2" t="n">
-        <v>46045</v>
+        <v>46041</v>
       </c>
       <c r="B379" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
         </is>
       </c>
       <c r="C379" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="D379" s="3" t="inlineStr">
         <is>
-          <t>16811</t>
+          <t>58310926</t>
         </is>
       </c>
       <c r="E379" s="3" t="inlineStr">
         <is>
-          <t>Vace Varasteh per diem Per diem for week of 1/26/2026 - 2/21/2026</t>
+          <t>Shipping</t>
         </is>
       </c>
       <c r="F379" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="G379" s="4" t="n">
-        <v>350</v>
+        <v>16.44</v>
       </c>
       <c r="H379" s="5" t="n">
         <v>500</v>
@@ -16802,38 +16822,2044 @@
     </row>
     <row r="380">
       <c r="A380" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B380" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C380" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D380" s="3" t="inlineStr">
+        <is>
+          <t>58542308</t>
+        </is>
+      </c>
+      <c r="E380" s="3" t="inlineStr">
+        <is>
+          <t>Felt Filter Bag for Water, Sewn Seam, 7" Diameter</t>
+        </is>
+      </c>
+      <c r="F380" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G380" s="4" t="n">
+        <v>228.25</v>
+      </c>
+      <c r="H380" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B381" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C381" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D381" s="3" t="inlineStr">
+        <is>
+          <t>58542308</t>
+        </is>
+      </c>
+      <c r="E381" s="3" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F381" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G381" s="4" t="n">
+        <v>17.69</v>
+      </c>
+      <c r="H381" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B382" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C382" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D382" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E382" s="3" t="inlineStr">
+        <is>
+          <t>2 LONG RADIUS 45 ELBOW WELD HEAT</t>
+        </is>
+      </c>
+      <c r="F382" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G382" s="4" t="n">
+        <v>84.95999999999999</v>
+      </c>
+      <c r="H382" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B383" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C383" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D383" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E383" s="3" t="inlineStr">
+        <is>
+          <t>WLDCAP2</t>
+        </is>
+      </c>
+      <c r="F383" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G383" s="4" t="n">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="H383" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B384" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C384" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D384" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E384" s="3" t="inlineStr">
+        <is>
+          <t>2 LONG RADIUS 90 ELBOW WELD HEAT</t>
+        </is>
+      </c>
+      <c r="F384" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G384" s="4" t="n">
+        <v>265.65</v>
+      </c>
+      <c r="H384" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B385" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C385" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D385" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E385" s="3" t="inlineStr">
+        <is>
+          <t>2 150# RF SLIP-ON WELD FLANGE A105 HEAT</t>
+        </is>
+      </c>
+      <c r="F385" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G385" s="4" t="n">
+        <v>202.6</v>
+      </c>
+      <c r="H385" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B386" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C386" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D386" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E386" s="3" t="inlineStr">
+        <is>
+          <t>2 150# 1/16 FULL FACE GASKET NON-ASBESTOS FIBER</t>
+        </is>
+      </c>
+      <c r="F386" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G386" s="4" t="n">
+        <v>60</v>
+      </c>
+      <c r="H386" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B387" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C387" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D387" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E387" s="3" t="inlineStr">
+        <is>
+          <t>2 - 3 BOLT SET PLTD 307A (4) 5/8 X 3</t>
+        </is>
+      </c>
+      <c r="F387" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G387" s="4" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="H387" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B388" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C388" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D388" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E388" s="3" t="inlineStr">
+        <is>
+          <t>2 TEE WELD HEAT</t>
+        </is>
+      </c>
+      <c r="F388" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G388" s="4" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="H388" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B389" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C389" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D389" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E389" s="3" t="inlineStr">
+        <is>
+          <t>tax</t>
+        </is>
+      </c>
+      <c r="F389" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G389" s="4" t="n">
+        <v>99.51000000000001</v>
+      </c>
+      <c r="H389" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B390" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C390" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D390" s="3" t="inlineStr">
+        <is>
+          <t>252549305-006</t>
+        </is>
+      </c>
+      <c r="E390" s="3" t="inlineStr">
+        <is>
+          <t>375/0525 FENCE MODULAR 12' L X 6' H TEMPORARY PAN</t>
+        </is>
+      </c>
+      <c r="F390" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G390" s="4" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="H390" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B391" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C391" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D391" s="3" t="inlineStr">
+        <is>
+          <t>252549305-006</t>
+        </is>
+      </c>
+      <c r="E391" s="3" t="inlineStr">
+        <is>
+          <t>Fence Wheel and weight</t>
+        </is>
+      </c>
+      <c r="F391" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G391" s="4" t="n">
+        <v>65</v>
+      </c>
+      <c r="H391" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B392" s="3" t="inlineStr">
+        <is>
+          <t>5115 · Rent - Equipment (direct)</t>
+        </is>
+      </c>
+      <c r="C392" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D392" s="3" t="inlineStr">
+        <is>
+          <t>252549305-006</t>
+        </is>
+      </c>
+      <c r="E392" s="3" t="inlineStr">
+        <is>
+          <t>Service Charge and Tax</t>
+        </is>
+      </c>
+      <c r="F392" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G392" s="4" t="n">
+        <v>12.56</v>
+      </c>
+      <c r="H392" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B393" s="3" t="inlineStr">
+        <is>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
+        </is>
+      </c>
+      <c r="C393" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D393" s="3" t="inlineStr">
+        <is>
+          <t>58542308</t>
+        </is>
+      </c>
+      <c r="E393" s="3" t="inlineStr">
+        <is>
+          <t>Shipping</t>
+        </is>
+      </c>
+      <c r="F393" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G393" s="4" t="n">
+        <v>20.23</v>
+      </c>
+      <c r="H393" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B394" s="3" t="inlineStr">
+        <is>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
+        </is>
+      </c>
+      <c r="C394" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D394" s="3" t="inlineStr">
+        <is>
+          <t>1611105730</t>
+        </is>
+      </c>
+      <c r="E394" s="3" t="inlineStr">
+        <is>
+          <t>Shipping</t>
+        </is>
+      </c>
+      <c r="F394" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G394" s="4" t="n">
+        <v>124.87</v>
+      </c>
+      <c r="H394" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="2" t="n">
         <v>46045</v>
       </c>
-      <c r="B380" s="3" t="inlineStr">
+      <c r="B395" s="3" t="inlineStr">
         <is>
           <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
-      <c r="C380" s="3" t="inlineStr">
+      <c r="C395" s="3" t="inlineStr">
         <is>
           <t>General Journal</t>
         </is>
       </c>
-      <c r="D380" s="3" t="inlineStr">
+      <c r="D395" s="3" t="inlineStr">
         <is>
           <t>16811</t>
         </is>
       </c>
-      <c r="E380" s="3" t="inlineStr">
+      <c r="E395" s="3" t="inlineStr">
+        <is>
+          <t>Luke Giguere per diem Per diem for week of 1/26/2026 - 2/21/2026</t>
+        </is>
+      </c>
+      <c r="F395" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G395" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H395" s="5" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="2" t="n">
+        <v>46045</v>
+      </c>
+      <c r="B396" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C396" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D396" s="3" t="inlineStr">
+        <is>
+          <t>16811</t>
+        </is>
+      </c>
+      <c r="E396" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt per diem Per diem for week of 1/26/2026 - 2/21/2026</t>
+        </is>
+      </c>
+      <c r="F396" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G396" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H396" s="5" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="2" t="n">
+        <v>46045</v>
+      </c>
+      <c r="B397" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C397" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D397" s="3" t="inlineStr">
+        <is>
+          <t>16811</t>
+        </is>
+      </c>
+      <c r="E397" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt per diem Per diem for week of 1/17/2026 - 1/18/2026</t>
+        </is>
+      </c>
+      <c r="F397" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G397" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H397" s="5" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="2" t="n">
+        <v>46045</v>
+      </c>
+      <c r="B398" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C398" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D398" s="3" t="inlineStr">
+        <is>
+          <t>16811</t>
+        </is>
+      </c>
+      <c r="E398" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh per diem Per diem for week of 1/26/2026 - 2/21/2026</t>
+        </is>
+      </c>
+      <c r="F398" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G398" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H398" s="5" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="2" t="n">
+        <v>46045</v>
+      </c>
+      <c r="B399" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C399" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D399" s="3" t="inlineStr">
+        <is>
+          <t>16811</t>
+        </is>
+      </c>
+      <c r="E399" s="3" t="inlineStr">
         <is>
           <t>Vace Varasteh per diem Per diem for week of 1/9/2026 - 1/11/2026</t>
         </is>
       </c>
-      <c r="F380" s="3" t="inlineStr">
+      <c r="F399" s="3" t="inlineStr">
         <is>
           <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
-      <c r="G380" s="4" t="n">
+      <c r="G399" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="H380" s="5" t="n">
+      <c r="H399" s="5" t="n">
         <v>500</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="2" t="n">
+        <v>46048</v>
+      </c>
+      <c r="B400" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C400" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D400" s="3" t="inlineStr">
+        <is>
+          <t>9784026081</t>
+        </is>
+      </c>
+      <c r="E400" s="3" t="inlineStr">
+        <is>
+          <t>GATE VALVE,1",BRASS,NPT</t>
+        </is>
+      </c>
+      <c r="F400" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G400" s="4" t="n">
+        <v>2022.75</v>
+      </c>
+      <c r="H400" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="2" t="n">
+        <v>46048</v>
+      </c>
+      <c r="B401" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C401" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D401" s="3" t="inlineStr">
+        <is>
+          <t>9784026081</t>
+        </is>
+      </c>
+      <c r="E401" s="3" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F401" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G401" s="4" t="n">
+        <v>189.64</v>
+      </c>
+      <c r="H401" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="2" t="n">
+        <v>46051</v>
+      </c>
+      <c r="B402" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C402" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D402" s="3" t="inlineStr">
+        <is>
+          <t>1611105730-1</t>
+        </is>
+      </c>
+      <c r="E402" s="3" t="inlineStr">
+        <is>
+          <t>2 CAP WELD HEAT</t>
+        </is>
+      </c>
+      <c r="F402" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G402" s="4" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="H402" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="2" t="n">
+        <v>46051</v>
+      </c>
+      <c r="B403" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C403" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D403" s="3" t="inlineStr">
+        <is>
+          <t>1611105730-1</t>
+        </is>
+      </c>
+      <c r="E403" s="3" t="inlineStr">
+        <is>
+          <t>2 150# RF SLIP-ON WELD FLANGE A105 HEAT</t>
+        </is>
+      </c>
+      <c r="F403" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G403" s="4" t="n">
+        <v>526.76</v>
+      </c>
+      <c r="H403" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="2" t="n">
+        <v>46051</v>
+      </c>
+      <c r="B404" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C404" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D404" s="3" t="inlineStr">
+        <is>
+          <t>1611105730-1</t>
+        </is>
+      </c>
+      <c r="E404" s="3" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F404" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G404" s="4" t="n">
+        <v>50.73</v>
+      </c>
+      <c r="H404" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="2" t="n">
+        <v>46052</v>
+      </c>
+      <c r="B405" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C405" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D405" s="3" t="inlineStr">
+        <is>
+          <t>IN222703</t>
+        </is>
+      </c>
+      <c r="E405" s="3" t="inlineStr">
+        <is>
+          <t>10' galv spiral pipe 1- ft 26 ga</t>
+        </is>
+      </c>
+      <c r="F405" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G405" s="4" t="n">
+        <v>1925</v>
+      </c>
+      <c r="H405" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="2" t="n">
+        <v>46055</v>
+      </c>
+      <c r="B406" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C406" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D406" s="3" t="inlineStr">
+        <is>
+          <t>16815</t>
+        </is>
+      </c>
+      <c r="E406" s="3" t="inlineStr">
+        <is>
+          <t>Luke Giguere Per diem for week of 2/2/2026 - 2/8/2026</t>
+        </is>
+      </c>
+      <c r="F406" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G406" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H406" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="2" t="n">
+        <v>46055</v>
+      </c>
+      <c r="B407" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C407" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D407" s="3" t="inlineStr">
+        <is>
+          <t>16815</t>
+        </is>
+      </c>
+      <c r="E407" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt Per diem for week of 2/2/2026 - 2/8/2026</t>
+        </is>
+      </c>
+      <c r="F407" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G407" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H407" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="2" t="n">
+        <v>46055</v>
+      </c>
+      <c r="B408" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C408" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D408" s="3" t="inlineStr">
+        <is>
+          <t>16815</t>
+        </is>
+      </c>
+      <c r="E408" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh Per diem for week of 2/2/2026 - 2/8/2026</t>
+        </is>
+      </c>
+      <c r="F408" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G408" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H408" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B409" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C409" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D409" s="3" t="inlineStr">
+        <is>
+          <t>1611148835</t>
+        </is>
+      </c>
+      <c r="E409" s="3" t="inlineStr">
+        <is>
+          <t>2 BLK PE A53B SCH40 STEEL PIPE .154W HEAT</t>
+        </is>
+      </c>
+      <c r="F409" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G409" s="4" t="n">
+        <v>745.9</v>
+      </c>
+      <c r="H409" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B410" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C410" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D410" s="3" t="inlineStr">
+        <is>
+          <t>1611148835</t>
+        </is>
+      </c>
+      <c r="E410" s="3" t="inlineStr">
+        <is>
+          <t>2 LONG RADIUS 45 ELBOW WELD HEAT</t>
+        </is>
+      </c>
+      <c r="F410" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G410" s="4" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="H410" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B411" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C411" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D411" s="3" t="inlineStr">
+        <is>
+          <t>1611148835</t>
+        </is>
+      </c>
+      <c r="E411" s="3" t="inlineStr">
+        <is>
+          <t>2 150# RF SLIP-ON WELD FLANGE A105 HEAT</t>
+        </is>
+      </c>
+      <c r="F411" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G411" s="4" t="n">
+        <v>14.66</v>
+      </c>
+      <c r="H411" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B412" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C412" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D412" s="3" t="inlineStr">
+        <is>
+          <t>1611148835</t>
+        </is>
+      </c>
+      <c r="E412" s="3" t="inlineStr">
+        <is>
+          <t>2 150# 1/16 FULL FACE GASKET NON-ASBESTOS FIBER</t>
+        </is>
+      </c>
+      <c r="F412" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G412" s="4" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="H412" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B413" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C413" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D413" s="3" t="inlineStr">
+        <is>
+          <t>1611148835</t>
+        </is>
+      </c>
+      <c r="E413" s="3" t="inlineStr">
+        <is>
+          <t>2 - 3 BOLT SET PLTD 307A (4) 5/8 X 3</t>
+        </is>
+      </c>
+      <c r="F413" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G413" s="4" t="n">
+        <v>13.84</v>
+      </c>
+      <c r="H413" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B414" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C414" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D414" s="3" t="inlineStr">
+        <is>
+          <t>1611148835</t>
+        </is>
+      </c>
+      <c r="E414" s="3" t="inlineStr">
+        <is>
+          <t>tax</t>
+        </is>
+      </c>
+      <c r="F414" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G414" s="4" t="n">
+        <v>73.88</v>
+      </c>
+      <c r="H414" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B415" s="3" t="inlineStr">
+        <is>
+          <t>5112 · Carbon &amp; Lab Samplies (Driect)</t>
+        </is>
+      </c>
+      <c r="C415" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D415" s="3" t="inlineStr">
+        <is>
+          <t>CSI 134-26</t>
+        </is>
+      </c>
+      <c r="E415" s="3" t="inlineStr">
+        <is>
+          <t>55 Gallon Liquid Phase Filter Drums filled with Liquid Phase Coconut Shell Activated Carbon</t>
+        </is>
+      </c>
+      <c r="F415" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G415" s="4" t="n">
+        <v>2600</v>
+      </c>
+      <c r="H415" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="2" t="n">
+        <v>46057</v>
+      </c>
+      <c r="B416" s="3" t="inlineStr">
+        <is>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
+        </is>
+      </c>
+      <c r="C416" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D416" s="3" t="inlineStr">
+        <is>
+          <t>CSI 134-26</t>
+        </is>
+      </c>
+      <c r="E416" s="3" t="inlineStr">
+        <is>
+          <t>Shipping</t>
+        </is>
+      </c>
+      <c r="F416" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G416" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H416" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B417" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C417" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D417" s="3" t="inlineStr">
+        <is>
+          <t>16818</t>
+        </is>
+      </c>
+      <c r="E417" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt Per diem for week of 2/9/2026 - 2/15/2026</t>
+        </is>
+      </c>
+      <c r="F417" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G417" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H417" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B418" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C418" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D418" s="3" t="inlineStr">
+        <is>
+          <t>16818</t>
+        </is>
+      </c>
+      <c r="E418" s="3" t="inlineStr">
+        <is>
+          <t>Mike Cogswell Per diem for week of 2/9/2026 - 2/15/2026</t>
+        </is>
+      </c>
+      <c r="F418" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G418" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="H418" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B419" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C419" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D419" s="3" t="inlineStr">
+        <is>
+          <t>16818</t>
+        </is>
+      </c>
+      <c r="E419" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh Per diem for week of 2/9/2026 - 2/15/2026</t>
+        </is>
+      </c>
+      <c r="F419" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G419" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H419" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B420" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C420" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D420" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E420" s="3" t="inlineStr">
+        <is>
+          <t>3 LONG RADIUS 90 ELBOW WELD HEAT</t>
+        </is>
+      </c>
+      <c r="F420" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G420" s="4" t="n">
+        <v>258.15</v>
+      </c>
+      <c r="H420" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B421" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C421" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D421" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E421" s="3" t="inlineStr">
+        <is>
+          <t>2 150# RF SLIP-ON WELD FLANGE A105 HEAT</t>
+        </is>
+      </c>
+      <c r="F421" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G421" s="4" t="n">
+        <v>14.66</v>
+      </c>
+      <c r="H421" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B422" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C422" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D422" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E422" s="3" t="inlineStr">
+        <is>
+          <t>3 150# RF SLIP-ON WELD FLANGE A105 HEAT</t>
+        </is>
+      </c>
+      <c r="F422" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G422" s="4" t="n">
+        <v>274.56</v>
+      </c>
+      <c r="H422" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B423" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C423" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D423" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E423" s="3" t="inlineStr">
+        <is>
+          <t>6 150# RF SLIP-ON WELD FLANGE A105 HEAT</t>
+        </is>
+      </c>
+      <c r="F423" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G423" s="4" t="n">
+        <v>285.6</v>
+      </c>
+      <c r="H423" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B424" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C424" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D424" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E424" s="3" t="inlineStr">
+        <is>
+          <t>3 150# 1/16 FULL FACE GASKET NON-ASBESTOS FIBER</t>
+        </is>
+      </c>
+      <c r="F424" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G424" s="4" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="H424" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B425" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C425" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D425" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E425" s="3" t="inlineStr">
+        <is>
+          <t>6 150# 1/16 FULL FACE GASKET NON-ASBESTOS FIBER</t>
+        </is>
+      </c>
+      <c r="F425" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G425" s="4" t="n">
+        <v>37.04</v>
+      </c>
+      <c r="H425" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B426" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C426" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D426" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E426" s="3" t="inlineStr">
+        <is>
+          <t>6 BOLT SET PLTD 307A (8) 3/4 X 3 1/4</t>
+        </is>
+      </c>
+      <c r="F426" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G426" s="4" t="n">
+        <v>173.96</v>
+      </c>
+      <c r="H426" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B427" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C427" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D427" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E427" s="3" t="inlineStr">
+        <is>
+          <t>2 - 3 BOLT SET PLTD 307A (4) 5/8 X 3</t>
+        </is>
+      </c>
+      <c r="F427" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G427" s="4" t="n">
+        <v>83.04000000000001</v>
+      </c>
+      <c r="H427" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B428" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C428" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D428" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E428" s="3" t="inlineStr">
+        <is>
+          <t>6 X 3 CONC REDUCER WELD HEAT</t>
+        </is>
+      </c>
+      <c r="F428" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G428" s="4" t="n">
+        <v>29.73</v>
+      </c>
+      <c r="H428" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B429" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="C429" s="3" t="inlineStr">
+        <is>
+          <t>Bill</t>
+        </is>
+      </c>
+      <c r="D429" s="3" t="inlineStr">
+        <is>
+          <t>1611156933</t>
+        </is>
+      </c>
+      <c r="E429" s="3" t="inlineStr">
+        <is>
+          <t>tax</t>
+        </is>
+      </c>
+      <c r="F429" s="3" t="inlineStr">
+        <is>
+          <t>2000 · Accounts Payable</t>
+        </is>
+      </c>
+      <c r="G429" s="4" t="n">
+        <v>110.9</v>
+      </c>
+      <c r="H429" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="B430" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C430" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D430" s="3" t="inlineStr">
+        <is>
+          <t>16821</t>
+        </is>
+      </c>
+      <c r="E430" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh Per diem for week of 2/16/2026 - 2/22/2026</t>
+        </is>
+      </c>
+      <c r="F430" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G430" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H430" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="2" t="n">
+        <v>46065</v>
+      </c>
+      <c r="B431" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C431" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D431" s="3" t="inlineStr">
+        <is>
+          <t>16821</t>
+        </is>
+      </c>
+      <c r="E431" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt Per diem for week of 2/16/2026 - 2/22/2026</t>
+        </is>
+      </c>
+      <c r="F431" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G431" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H431" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="2" t="n">
+        <v>46073</v>
+      </c>
+      <c r="B432" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C432" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D432" s="3" t="inlineStr">
+        <is>
+          <t>16822</t>
+        </is>
+      </c>
+      <c r="E432" s="3" t="inlineStr">
+        <is>
+          <t>Michael Hyatt Per diem for week of 2/23/2026 - 3/1/2026</t>
+        </is>
+      </c>
+      <c r="F432" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G432" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H432" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="2" t="n">
+        <v>46073</v>
+      </c>
+      <c r="B433" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="C433" s="3" t="inlineStr">
+        <is>
+          <t>General Journal</t>
+        </is>
+      </c>
+      <c r="D433" s="3" t="inlineStr">
+        <is>
+          <t>16822</t>
+        </is>
+      </c>
+      <c r="E433" s="3" t="inlineStr">
+        <is>
+          <t>Vace Varasteh Per diem for week of 2/23/2026 - 3/1/2026</t>
+        </is>
+      </c>
+      <c r="F433" s="3" t="inlineStr">
+        <is>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+        </is>
+      </c>
+      <c r="G433" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="H433" s="5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>